<commit_message>
Updated graphs in xlsx and presentation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Grad1\Randomized\RandomizedProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97D7E7F-2425-445F-805E-942C3DA65B6A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293702B3-E21E-4183-8856-1AD1D2A4B1D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8628" windowHeight="312" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="27">
   <si>
     <t>input_small_gen.txt</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>random 90%</t>
+  </si>
+  <si>
+    <t>boundary</t>
   </si>
 </sst>
 </file>
@@ -2715,6 +2718,92 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>boundary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>has_one</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>missing_one</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EA19-4A06-BAE4-ADA02C05F646}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3475,6 +3564,92 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-1C25-465E-B8C8-762D0076BA1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>boundary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$1:$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>random 10%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>random 25%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>random 50%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>random 75%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>random 90%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB85-4923-8998-0F676E954FE6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16823,8 +16998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="109" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="109" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -17090,6 +17265,42 @@
       <c r="B6">
         <v>0.66666666666666663</v>
       </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">

</xml_diff>